<commit_message>
add data file, finish tests
</commit_message>
<xml_diff>
--- a/idaes/dmf/tests/data_files/tables_data.xlsx
+++ b/idaes/dmf/tests/data_files/tables_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanGunter\src\idaes\dangunter\idaes-pse\idaes\dmf\tests\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F9877C6-C42D-472B-905C-1C7354ED2F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8360E414-D604-4429-88C1-DDBFA6AA3996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16060" yWindow="6610" windowWidth="21600" windowHeight="12680" xr2:uid="{780E5F8D-CB50-4563-8860-7357405EDC5F}"/>
+    <workbookView xWindow="10755" yWindow="5797" windowWidth="16200" windowHeight="9510" xr2:uid="{780E5F8D-CB50-4563-8860-7357405EDC5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>C2 (mol/L)</t>
-  </si>
-  <si>
-    <t>C1 (m/s)</t>
   </si>
   <si>
     <t>C3 (m^3/kg)</t>
@@ -48,13 +45,22 @@
   <si>
     <t>C2-1 (m/s)</t>
   </si>
+  <si>
+    <t>C1 [m/s]</t>
+  </si>
+  <si>
+    <t>C2 [mol/L]</t>
+  </si>
+  <si>
+    <t>C3 [(m^3)/kg]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -97,7 +103,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,27 +421,27 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.90625" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="1" max="1" width="12.9296875" customWidth="1"/>
+    <col min="2" max="2" width="14.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -446,7 +452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -471,20 +477,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -495,7 +501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>

</xml_diff>